<commit_message>
Add analysis for week 7-Sep to 11-Sep 2025
 New Week Statistics:
- Total Students: 449 (+10 from previous week)
- Full Week Attendance: 118 students (26.3%)
- Partial Attendance: 198 students (44.1%)
- Never Attended: 133 students (29.6%)
- Average Attendance: 52.7% (+4.1% improvement)
- Groups Analyzed: 20 (unchanged)

 Technical Improvements:
- DEYE group properly refined (no longer inflated count)
- Multi-week system successfully handling second week
- Master dashboard updated with week selection cards
- All reports and visualizations generated

 Files Generated:
- weeks/week_7Sep-11Sep/dashboard_week_7Sep-11Sep.html
- weeks/week_7Sep-11Sep/attendance_report_week_7Sep-11Sep.xlsx
- weeks/week_7Sep-11Sep/group_distribution.png
- weeks/week_7Sep-11Sep/overall_distribution.png
- Updated master_dashboard.html with 2-week selection
</commit_message>
<xml_diff>
--- a/weeks/week_31Aug-4Sep/weekly_attendance_results_31Aug-4Sep.xlsx
+++ b/weeks/week_31Aug-4Sep/weekly_attendance_results_31Aug-4Sep.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Black Gold\attendance statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Black Gold\attendance statistics\weeks\week_31Aug-4Sep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF8BCF4-F2D1-4AEA-98DC-BDD29D3190AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C6A946-65DC-4C0D-9FB5-8381F44F9B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1708,34 +1708,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1779,7 +1752,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1809,7 +1781,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1828,6 +1799,49 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1843,59 +1857,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
@@ -2012,8 +1973,15 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <name val="Calibri"/>
+        <family val="2"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2024,8 +1992,15 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <name val="Calibri"/>
+        <family val="2"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2041,9 +2016,10 @@
         <sz val="12"/>
         <color auto="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
@@ -2476,6 +2452,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2486,6 +2469,13 @@
         <name val="Calibri"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2660,11 +2650,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2674,18 +2669,16 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2695,24 +2688,31 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
+        </left>
+        <right style="thin">
           <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -2729,60 +2729,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5AC0BAD-DE2F-45AD-90B4-180AC6F7FD92}" name="Table1" displayName="Table1" ref="A1:F22" totalsRowCount="1" headerRowDxfId="61" dataDxfId="59" totalsRowDxfId="60" headerRowBorderDxfId="80" tableBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5AC0BAD-DE2F-45AD-90B4-180AC6F7FD92}" name="Table1" displayName="Table1" ref="A1:F22" totalsRowCount="1" headerRowDxfId="81" dataDxfId="79" totalsRowDxfId="77" headerRowBorderDxfId="80" tableBorderDxfId="78">
   <autoFilter ref="A1:F21" xr:uid="{F5AC0BAD-DE2F-45AD-90B4-180AC6F7FD92}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{05BB5593-38D3-4D61-A727-D5226B9630D6}" name="Group" totalsRowLabel="Total" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{061AEB9B-2B6D-4B5D-B31D-D74807A06821}" name="Total Students" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{E18C3364-A86C-45A4-90D3-994D38A4B2F6}" name="Full Week (5/5)" totalsRowFunction="custom" dataDxfId="69" totalsRowDxfId="68">
+    <tableColumn id="1" xr3:uid="{05BB5593-38D3-4D61-A727-D5226B9630D6}" name="Group" totalsRowLabel="Total" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{061AEB9B-2B6D-4B5D-B31D-D74807A06821}" name="Total Students" totalsRowFunction="sum" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{E18C3364-A86C-45A4-90D3-994D38A4B2F6}" name="Full Week (5/5)" totalsRowFunction="custom" dataDxfId="72" totalsRowDxfId="71">
       <totalsRowFormula>SUM(C1:C21)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DB804C0A-9C87-48F8-A3A3-4203C98AD8D2}" name="Partial (1-4)" totalsRowFunction="custom" dataDxfId="67" totalsRowDxfId="66">
+    <tableColumn id="4" xr3:uid="{DB804C0A-9C87-48F8-A3A3-4203C98AD8D2}" name="Partial (1-4)" totalsRowFunction="custom" dataDxfId="70" totalsRowDxfId="69">
       <totalsRowFormula>SUM(D1:D21)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{EA33B283-B171-46F2-A5A9-1C17CF27B894}" name="Never Attended" totalsRowFunction="custom" dataDxfId="65" totalsRowDxfId="64">
+    <tableColumn id="5" xr3:uid="{EA33B283-B171-46F2-A5A9-1C17CF27B894}" name="Never Attended" totalsRowFunction="custom" dataDxfId="68" totalsRowDxfId="67">
       <totalsRowFormula>SUM(E1:E21)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9C9AB255-BD44-4257-8A09-C48F8D4223EE}" name="Average Attendance %" totalsRowFunction="average" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{9C9AB255-BD44-4257-8A09-C48F8D4223EE}" name="Average Attendance %" totalsRowFunction="average" dataDxfId="66" totalsRowDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DF63B61-3304-4AA9-B18F-16A57479614E}" name="Table2" displayName="Table2" ref="A1:Q441" totalsRowCount="1" headerRowDxfId="24" dataDxfId="22" totalsRowDxfId="23" headerRowBorderDxfId="78" tableBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9DF63B61-3304-4AA9-B18F-16A57479614E}" name="Table2" displayName="Table2" ref="A1:Q441" totalsRowCount="1" headerRowDxfId="64" dataDxfId="62" totalsRowDxfId="60" headerRowBorderDxfId="63" tableBorderDxfId="61">
   <autoFilter ref="A1:Q440" xr:uid="{9DF63B61-3304-4AA9-B18F-16A57479614E}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{60F98823-4DDB-49F5-8CA6-E680A1020EC2}" name="Group" totalsRowLabel="Total" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{0247CDE9-9CDC-44A7-B6A5-E491ED65916F}" name="Student Number" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{74DA7FEE-0D56-4828-8B3D-E7824311E82A}" name="Student Name" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{0A08E2E9-7806-42A9-B8FD-28B6F1A0717D}" name="Student ID" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{A0ACE913-0407-474F-A6F6-B01145CFC208}" name="Days Attended" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{FD6DF71F-C4C0-48E1-9E2C-8263604E47D3}" name="Attendance %" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{CAD8D40A-54F9-4F7E-BC32-579A157EC05F}" name="Total Sessions" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{9EF2920A-41BB-414B-8CC0-279C1C465B5B}" name="Sun (31-Aug)" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{FDC731B1-B306-4008-A68C-71FBA6FDE15F}" name="Mon (1-Sep)" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="10" xr3:uid="{D8FE9C40-A974-4483-B611-7A20336A9462}" name="Tue (2-Sep)" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{3C7B4A3B-700C-448B-94D9-D7DF48302066}" name="Wed (3-Sep)" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="12" xr3:uid="{90597D01-70EC-4ECE-BD19-9DC963ACDDC3}" name="Thu (4-Sep)" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{86A9F4FA-FD05-4951-8D80-6FF93420F148}" name="Sun Sessions" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="14" xr3:uid="{7E35B90C-CCE8-4DFA-A73B-8D85BFE73D76}" name="Mon Sessions" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="15" xr3:uid="{865A2DB8-622D-4FCD-9B38-EB11A88E5C7C}" name="Tue Sessions" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="16" xr3:uid="{5E4BDF7C-D61E-4726-B3E6-7BB0EED22A06}" name="Wed Sessions" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="17" xr3:uid="{A5B0B278-05B0-46A6-B23F-883235106AC2}" name="Thu Sessions" totalsRowFunction="count" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{60F98823-4DDB-49F5-8CA6-E680A1020EC2}" name="Group" totalsRowLabel="Total" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{0247CDE9-9CDC-44A7-B6A5-E491ED65916F}" name="Student Number" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{74DA7FEE-0D56-4828-8B3D-E7824311E82A}" name="Student Name" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{0A08E2E9-7806-42A9-B8FD-28B6F1A0717D}" name="Student ID" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{A0ACE913-0407-474F-A6F6-B01145CFC208}" name="Days Attended" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{FD6DF71F-C4C0-48E1-9E2C-8263604E47D3}" name="Attendance %" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{CAD8D40A-54F9-4F7E-BC32-579A157EC05F}" name="Total Sessions" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{9EF2920A-41BB-414B-8CC0-279C1C465B5B}" name="Sun (31-Aug)" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="9" xr3:uid="{FDC731B1-B306-4008-A68C-71FBA6FDE15F}" name="Mon (1-Sep)" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{D8FE9C40-A974-4483-B611-7A20336A9462}" name="Tue (2-Sep)" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="11" xr3:uid="{3C7B4A3B-700C-448B-94D9-D7DF48302066}" name="Wed (3-Sep)" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{90597D01-70EC-4ECE-BD19-9DC963ACDDC3}" name="Thu (4-Sep)" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="13" xr3:uid="{86A9F4FA-FD05-4951-8D80-6FF93420F148}" name="Sun Sessions" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="14" xr3:uid="{7E35B90C-CCE8-4DFA-A73B-8D85BFE73D76}" name="Mon Sessions" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="15" xr3:uid="{865A2DB8-622D-4FCD-9B38-EB11A88E5C7C}" name="Tue Sessions" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{5E4BDF7C-D61E-4726-B3E6-7BB0EED22A06}" name="Wed Sessions" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="17" xr3:uid="{A5B0B278-05B0-46A6-B23F-883235106AC2}" name="Thu Sessions" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{049DE991-0491-4B68-8FFE-5F7D619F84C6}" name="Table3" displayName="Table3" ref="A1:D97" totalsRowCount="1" headerRowDxfId="13" dataDxfId="11" totalsRowDxfId="12" headerRowBorderDxfId="76" tableBorderDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{049DE991-0491-4B68-8FFE-5F7D619F84C6}" name="Table3" displayName="Table3" ref="A1:D97" totalsRowCount="1" headerRowDxfId="25" dataDxfId="23" totalsRowDxfId="21" headerRowBorderDxfId="24" tableBorderDxfId="22">
   <autoFilter ref="A1:D96" xr:uid="{049DE991-0491-4B68-8FFE-5F7D619F84C6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0DC72DA0-F35D-49C1-B670-FEF1BB134708}" name="Group" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{A374D83E-C4A9-4D89-98C2-033E2F856690}" name="Student Number" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{730673DC-E79C-428A-9682-B1387D8C63F0}" name="Student Name" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{BDBDFAE0-2831-4D40-9293-183FCD723D81}" name="Student ID" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="1" xr3:uid="{0DC72DA0-F35D-49C1-B670-FEF1BB134708}" name="Group" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{A374D83E-C4A9-4D89-98C2-033E2F856690}" name="Student Number" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{730673DC-E79C-428A-9682-B1387D8C63F0}" name="Student Name" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{BDBDFAE0-2831-4D40-9293-183FCD723D81}" name="Student ID" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="13">
       <totalsRowFormula>COUNT(Table3[Student ID])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2791,13 +2791,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{383A7B8F-3F5E-454F-B321-DC3421064242}" name="Table4" displayName="Table4" ref="A1:D134" totalsRowCount="1" headerRowDxfId="10" dataDxfId="5" totalsRowDxfId="0" headerRowBorderDxfId="74" tableBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{383A7B8F-3F5E-454F-B321-DC3421064242}" name="Table4" displayName="Table4" ref="A1:D134" totalsRowCount="1" headerRowDxfId="12" dataDxfId="10" totalsRowDxfId="8" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="A1:D133" xr:uid="{383A7B8F-3F5E-454F-B321-DC3421064242}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{815630BD-8C2A-4D05-B006-9E8B328011A2}" name="Group" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DC6105F5-E3A1-4B44-9CA4-429CF75B5609}" name="Student Number" dataDxfId="8" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E963EEF7-F30D-44FF-930A-493EBFD36229}" name="Student Name" dataDxfId="7" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{6B6CA3FB-1C6F-4967-932B-2027BA1F5697}" name="Student ID" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{815630BD-8C2A-4D05-B006-9E8B328011A2}" name="Group" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DC6105F5-E3A1-4B44-9CA4-429CF75B5609}" name="Student Number" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E963EEF7-F30D-44FF-930A-493EBFD36229}" name="Student Name" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{6B6CA3FB-1C6F-4967-932B-2027BA1F5697}" name="Student ID" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3090,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3099,7 +3099,7 @@
     <col min="1" max="1" width="14.05078125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.83984375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5234375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.68359375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.15625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -3589,8 +3589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q441"/>
   <sheetViews>
-    <sheetView topLeftCell="A265" workbookViewId="0">
-      <selection sqref="A1:Q441"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -28373,7 +28373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
       <selection activeCell="A114" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>